<commit_message>
Modify Test.py, Excel VBA for publicSetting input
</commit_message>
<xml_diff>
--- a/CyberSecurity.xlsx
+++ b/CyberSecurity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="IEF" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
   <si>
     <t>Telnet Pswd</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -38,19 +38,216 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>User</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet IP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TelIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>in_file_dir</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>eth1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pswd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack which IP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack fron which Interface</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ips</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestResult</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>192.168.128.99</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter-DPI</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-IPS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-DOS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter-IDS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter-DPI</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-IPS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.128.99</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack which IP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-IPS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.128.99</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet IP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>aaron</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Telnet Account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmoxa</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet Pswd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ips</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>eth1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack fron which Interface</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-DOS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.128.99</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack which IP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TelIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>User</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Telnet IP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TelIP</t>
+    <t>aaron</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet Account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pswd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dos</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter-IDS</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -58,31 +255,67 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>./../Replay/Rewrite</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>in_file_dir</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>eth1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack Type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dos</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
+    <t>Filter-IDS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaron</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter-IDS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pawd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmoxa</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet Pswd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>./../Lib/Replay/Rewrite</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-BruteForce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.128.99</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-BruteForce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Port</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaron</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-BruteForce</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -90,72 +323,27 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>User</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack which IP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtIP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack fron which Interface</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ips</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>All</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestResult</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Variable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.127.100</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.128.99</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.128.99</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Filter-DPI</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack-IPS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack-DOS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Filter-IDS</t>
+    <t>adminmoxa</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-BruteForce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack-BruteForce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Port</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pswd</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmoxa</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -601,10 +789,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -614,24 +802,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -640,7 +828,7 @@
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
@@ -649,43 +837,43 @@
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
@@ -694,10 +882,10 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -709,73 +897,73 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
@@ -784,10 +972,10 @@
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -799,79 +987,79 @@
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>3</v>
@@ -879,7 +1067,7 @@
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>2</v>
@@ -888,8 +1076,62 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="2">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -900,10 +1142,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表2"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -913,24 +1155,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -939,7 +1181,7 @@
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
@@ -948,16 +1190,16 @@
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -966,28 +1208,28 @@
         <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -996,199 +1238,253 @@
         <v>32</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>